<commit_message>
Make Scen_Par-SRV_DC_Demand.xlsx consistent with demand projections
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
+++ b/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6035190-FB67-461A-AD0A-6FA4AD3026A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D3C36-1066-4581-905B-D2A5BC39026A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -427,7 +427,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,6 +522,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -644,7 +651,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -702,6 +709,11 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -711,11 +723,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1829,12 +1837,12 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="10"/>
@@ -1918,11 +1926,11 @@
       <c r="A19" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="16"/>
@@ -1950,11 +1958,11 @@
       <c r="A20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="16"/>
@@ -2042,11 +2050,11 @@
       <c r="A23" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -2130,11 +2138,11 @@
       <c r="A26" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2250,11 +2258,11 @@
       <c r="A30" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="8"/>
@@ -2282,11 +2290,11 @@
       <c r="A31" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="8"/>
@@ -5007,8 +5015,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5056,7 +5064,7 @@
       <c r="B8">
         <v>2021</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>3.9929999999999999</v>
       </c>
       <c r="H8">
@@ -5070,9 +5078,9 @@
       <c r="B9">
         <v>2022</v>
       </c>
-      <c r="C9" s="27">
-        <f>($C$17-$C$8)/($B$17-$B$8)*(B9-$B$8)+$C$8</f>
-        <v>5.3826666666666663</v>
+      <c r="C9" s="30">
+        <f>17.1311/3.6</f>
+        <v>4.7586388888888891</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -5085,63 +5093,63 @@
       <c r="B10">
         <v>2023</v>
       </c>
-      <c r="C10" s="27">
-        <f t="shared" ref="C10:C16" si="0">($C$17-$C$8)/($B$17-$B$8)*(B10-$B$8)+$C$8</f>
-        <v>6.7723333333333331</v>
+      <c r="C10" s="24">
+        <f>($C$17-$C$9)/($B$17-$B$9)*(B10-$B$9)+$C$9</f>
+        <v>6.2263090277777779</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2024</v>
       </c>
-      <c r="C11" s="27">
-        <f t="shared" si="0"/>
-        <v>8.161999999999999</v>
+      <c r="C11" s="24">
+        <f t="shared" ref="C11:C16" si="0">($C$17-$C$9)/($B$17-$B$9)*(B11-$B$9)+$C$9</f>
+        <v>7.6939791666666668</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>2025</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="24">
         <f t="shared" si="0"/>
-        <v>9.5516666666666659</v>
+        <v>9.1616493055555566</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2026</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="24">
         <f t="shared" si="0"/>
-        <v>10.941333333333333</v>
+        <v>10.629319444444445</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2027</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="24">
         <f t="shared" si="0"/>
-        <v>12.331</v>
+        <v>12.096989583333333</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2028</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="24">
         <f t="shared" si="0"/>
-        <v>13.720666666666666</v>
+        <v>13.564659722222222</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2029</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="24">
         <f t="shared" si="0"/>
-        <v>15.110333333333333</v>
+        <v>15.032329861111112</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -5155,7 +5163,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5163,7 +5171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8BCD28-42D1-4065-A61D-99892D29F9FE}">
   <dimension ref="C3:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -5174,7 +5182,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>83</v>
       </c>
       <c r="D3" t="s">
@@ -5182,46 +5190,46 @@
       </c>
     </row>
     <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="25">
         <v>2021</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="25">
         <v>2022</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="25">
         <v>2023</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="25">
         <v>2024</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="25">
         <v>2025</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="25">
         <v>2026</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="25">
         <v>2027</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="25">
         <v>2028</v>
       </c>
-      <c r="O4" s="28">
+      <c r="O4" s="25">
         <v>2029</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="25">
         <v>2030</v>
       </c>
     </row>
@@ -5236,43 +5244,43 @@
       <c r="F5" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="23">
         <f>VLOOKUP(demand!G4,config!$B$8:$C$17,2,FALSE)*3.6</f>
         <v>14.3748</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="23">
         <f>VLOOKUP(demand!H4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>19.377599999999997</v>
-      </c>
-      <c r="I5" s="26">
+        <v>17.1311</v>
+      </c>
+      <c r="I5" s="23">
         <f>VLOOKUP(demand!I4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>24.380399999999998</v>
-      </c>
-      <c r="J5" s="26">
+        <v>22.4147125</v>
+      </c>
+      <c r="J5" s="23">
         <f>VLOOKUP(demand!J4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>29.383199999999999</v>
-      </c>
-      <c r="K5" s="26">
+        <v>27.698325000000001</v>
+      </c>
+      <c r="K5" s="23">
         <f>VLOOKUP(demand!K4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>34.385999999999996</v>
-      </c>
-      <c r="L5" s="26">
+        <v>32.981937500000008</v>
+      </c>
+      <c r="L5" s="23">
         <f>VLOOKUP(demand!L4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>39.388799999999996</v>
-      </c>
-      <c r="M5" s="26">
+        <v>38.265550000000005</v>
+      </c>
+      <c r="M5" s="23">
         <f>VLOOKUP(demand!M4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>44.391599999999997</v>
-      </c>
-      <c r="N5" s="26">
+        <v>43.549162500000001</v>
+      </c>
+      <c r="N5" s="23">
         <f>VLOOKUP(demand!N4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>49.394399999999997</v>
-      </c>
-      <c r="O5" s="26">
+        <v>48.832774999999998</v>
+      </c>
+      <c r="O5" s="23">
         <f>VLOOKUP(demand!O4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>54.397199999999998</v>
-      </c>
-      <c r="P5" s="26">
+        <v>54.116387500000002</v>
+      </c>
+      <c r="P5" s="23">
         <f>VLOOKUP(demand!P4,config!$B$8:$C$17,2,FALSE)*3.6</f>
         <v>59.4</v>
       </c>

</xml_diff>

<commit_message>
Use DC demand projections from GCS 2022
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
+++ b/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D3C36-1066-4581-905B-D2A5BC39026A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D29951B-FF93-47DE-8227-9FEAF117D37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>LimType</t>
   </si>
@@ -398,9 +398,6 @@
     <t>Specify data centre demand</t>
   </si>
   <si>
-    <t>~InputCell:1-3</t>
-  </si>
-  <si>
     <t>Demand, TWh</t>
   </si>
   <si>
@@ -417,6 +414,12 @@
   </si>
   <si>
     <t>SRVDCE-CS</t>
+  </si>
+  <si>
+    <t>TS_Filter</t>
+  </si>
+  <si>
+    <t>~InputCell:1-2</t>
   </si>
 </sst>
 </file>
@@ -714,6 +717,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -723,7 +727,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1837,12 +1840,12 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="10"/>
@@ -1926,11 +1929,11 @@
       <c r="A19" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="16"/>
@@ -1958,11 +1961,11 @@
       <c r="A20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="16"/>
@@ -2050,11 +2053,11 @@
       <c r="A23" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
@@ -2138,11 +2141,11 @@
       <c r="A26" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
@@ -2258,11 +2261,11 @@
       <c r="A30" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="8"/>
@@ -2290,11 +2293,11 @@
       <c r="A31" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="8"/>
@@ -5013,10 +5016,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:I17"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,7 +5033,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -5043,7 +5046,7 @@
         <v>64</v>
       </c>
       <c r="I6">
-        <v>2030</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -5051,13 +5054,14 @@
         <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>16.5</v>
+        <f>1995*8760/10^6</f>
+        <v>17.476199999999999</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -5071,22 +5075,17 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <v>8</v>
+        <f>1025*8760/10^6</f>
+        <v>8.9789999999999992</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2022</v>
       </c>
-      <c r="C9" s="30">
-        <f>17.1311/3.6</f>
-        <v>4.7586388888888891</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
+      <c r="C9" s="27">
+        <f>600*8760/10^6</f>
+        <v>5.2560000000000002</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -5094,8 +5093,8 @@
         <v>2023</v>
       </c>
       <c r="C10" s="24">
-        <f>($C$17-$C$9)/($B$17-$B$9)*(B10-$B$9)+$C$9</f>
-        <v>6.2263090277777779</v>
+        <f>($C$18-$C$9)/($B$18-$B$9)*(B10-$B$9)+$C$9</f>
+        <v>6.6138000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -5103,8 +5102,8 @@
         <v>2024</v>
       </c>
       <c r="C11" s="24">
-        <f t="shared" ref="C11:C16" si="0">($C$17-$C$9)/($B$17-$B$9)*(B11-$B$9)+$C$9</f>
-        <v>7.6939791666666668</v>
+        <f t="shared" ref="C11:C17" si="0">($C$18-$C$9)/($B$18-$B$9)*(B11-$B$9)+$C$9</f>
+        <v>7.9716000000000005</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -5113,7 +5112,7 @@
       </c>
       <c r="C12" s="24">
         <f t="shared" si="0"/>
-        <v>9.1616493055555566</v>
+        <v>9.3293999999999997</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -5122,7 +5121,7 @@
       </c>
       <c r="C13" s="24">
         <f t="shared" si="0"/>
-        <v>10.629319444444445</v>
+        <v>10.687200000000001</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -5131,7 +5130,7 @@
       </c>
       <c r="C14" s="24">
         <f t="shared" si="0"/>
-        <v>12.096989583333333</v>
+        <v>12.045</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -5140,7 +5139,7 @@
       </c>
       <c r="C15" s="24">
         <f t="shared" si="0"/>
-        <v>13.564659722222222</v>
+        <v>13.402799999999999</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -5149,16 +5148,25 @@
       </c>
       <c r="C16" s="24">
         <f t="shared" si="0"/>
-        <v>15.032329861111112</v>
+        <v>14.7606</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2030</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="24">
+        <f t="shared" si="0"/>
+        <v>16.118400000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2031</v>
+      </c>
+      <c r="C18" s="24">
         <f>VLOOKUP(B3,H7:I9,2,FALSE)</f>
-        <v>16.5</v>
+        <v>17.476199999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5169,10 +5177,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8BCD28-42D1-4065-A61D-99892D29F9FE}">
-  <dimension ref="C3:P5"/>
+  <dimension ref="C3:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,15 +5189,15 @@
     <col min="4" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C3" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>0</v>
       </c>
@@ -5197,7 +5205,7 @@
         <v>63</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>61</v>
@@ -5232,57 +5240,70 @@
       <c r="P4" s="25">
         <v>2030</v>
       </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="25">
+        <v>2031</v>
+      </c>
+      <c r="R4" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3,Regions!$D$3)</f>
         <v>IE,National</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="23">
-        <f>VLOOKUP(demand!G4,config!$B$8:$C$17,2,FALSE)*3.6</f>
+        <f>VLOOKUP(demand!G4,config!$B$8:$C$18,2,FALSE)*3.6</f>
         <v>14.3748</v>
       </c>
       <c r="H5" s="23">
-        <f>VLOOKUP(demand!H4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>17.1311</v>
+        <f>VLOOKUP(demand!H4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>18.921600000000002</v>
       </c>
       <c r="I5" s="23">
-        <f>VLOOKUP(demand!I4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>22.4147125</v>
+        <f>VLOOKUP(demand!I4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>23.80968</v>
       </c>
       <c r="J5" s="23">
-        <f>VLOOKUP(demand!J4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>27.698325000000001</v>
+        <f>VLOOKUP(demand!J4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>28.697760000000002</v>
       </c>
       <c r="K5" s="23">
-        <f>VLOOKUP(demand!K4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>32.981937500000008</v>
+        <f>VLOOKUP(demand!K4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>33.585839999999997</v>
       </c>
       <c r="L5" s="23">
-        <f>VLOOKUP(demand!L4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>38.265550000000005</v>
+        <f>VLOOKUP(demand!L4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>38.473920000000007</v>
       </c>
       <c r="M5" s="23">
-        <f>VLOOKUP(demand!M4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>43.549162500000001</v>
+        <f>VLOOKUP(demand!M4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>43.362000000000002</v>
       </c>
       <c r="N5" s="23">
-        <f>VLOOKUP(demand!N4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>48.832774999999998</v>
+        <f>VLOOKUP(demand!N4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>48.250079999999997</v>
       </c>
       <c r="O5" s="23">
-        <f>VLOOKUP(demand!O4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>54.116387500000002</v>
+        <f>VLOOKUP(demand!O4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>53.138159999999999</v>
       </c>
       <c r="P5" s="23">
-        <f>VLOOKUP(demand!P4,config!$B$8:$C$17,2,FALSE)*3.6</f>
-        <v>59.4</v>
+        <f>VLOOKUP(demand!P4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>58.026240000000008</v>
+      </c>
+      <c r="Q5" s="23">
+        <f>VLOOKUP(demand!Q4,config!$B$8:$C$18,2,FALSE)*3.6</f>
+        <v>62.914319999999996</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a very low DC growth scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
+++ b/SuppXLS/Scen_Par-SRV_DC_Demand.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D29951B-FF93-47DE-8227-9FEAF117D37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F39449A-4432-46D3-A3A0-4EF225BE3F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -419,7 +419,7 @@
     <t>TS_Filter</t>
   </si>
   <si>
-    <t>~InputCell:1-2</t>
+    <t>~InputCell:1-3</t>
   </si>
 </sst>
 </file>
@@ -5018,9 +5018,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5087,6 +5085,12 @@
         <f>600*8760/10^6</f>
         <v>5.2560000000000002</v>
       </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>6.65</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -5177,10 +5181,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8BCD28-42D1-4065-A61D-99892D29F9FE}">
-  <dimension ref="C3:R5"/>
+  <dimension ref="C3:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5189,7 +5193,7 @@
     <col min="4" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="26" t="s">
         <v>82</v>
       </c>
@@ -5197,7 +5201,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>0</v>
       </c>
@@ -5243,11 +5247,14 @@
       <c r="Q4" s="25">
         <v>2031</v>
       </c>
-      <c r="R4" s="25" t="s">
+      <c r="R4" s="25">
+        <v>0</v>
+      </c>
+      <c r="S4" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>85</v>
       </c>
@@ -5302,7 +5309,10 @@
         <f>VLOOKUP(demand!Q4,config!$B$8:$C$18,2,FALSE)*3.6</f>
         <v>62.914319999999996</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="23">
+        <v>5</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
     </row>

</xml_diff>